<commit_message>
tài liệu update, lấy ngày 29/09/2023
</commit_message>
<xml_diff>
--- a/KMWS03/KMWS03/Yêu cầu nhỏ lẻ/要件1_KDW003日別実績の修正_成果物一覧.xlsx
+++ b/KMWS03/KMWS03/Yêu cầu nhỏ lẻ/要件1_KDW003日別実績の修正_成果物一覧.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kazuya_ushigaki\Documents\12_TuanTeam\01設計\02_メタウォーター_代行確認\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.50.4\share\500_新構想開発\04_設計\00_JP⇒VN説明会\20230922_1490_メタウォーター対応\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4FA64DA-A54D-402B-B0AA-9DD3B46CD28B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94877A1A-61FE-456F-9F8F-EC1DD7B84261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="成果物一覧" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>パス</t>
     <phoneticPr fontId="1"/>
@@ -256,10 +256,15 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>画面設計書-KDW003-A-日別実績の修正.xlsx</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>\\192.168.50.4\share\500_新構想開発\04_設計\60_UI設計\K_就業\KDW_日別実績\KDW003_日別実績の修正\ver4～</t>
-  </si>
-  <si>
-    <t>画面設計書-KDW003-A-日別実績の修正.xlsx</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ver59</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1019,7 +1024,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
+      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.850000000000001" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1163,7 +1168,7 @@
       <c r="A13" s="8"/>
       <c r="B13" s="21"/>
       <c r="C13" s="17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D13" s="22"/>
       <c r="E13" s="20"/>
@@ -1173,12 +1178,14 @@
       <c r="A14" s="8"/>
       <c r="B14" s="21"/>
       <c r="C14" s="24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D14" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="2"/>
+      <c r="E14" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.4">
@@ -1193,14 +1200,14 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
-  <conditionalFormatting sqref="A2:B4 A6:B6 A10:B10 A12:B12 A15:B15">
+  <conditionalFormatting sqref="A2:B4 A12:B12 A15:B15">
     <cfRule type="expression" dxfId="3" priority="324">
       <formula>$A2&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A7:B9">
+  <conditionalFormatting sqref="A6:B10">
     <cfRule type="expression" dxfId="2" priority="95">
-      <formula>$A7&lt;&gt;""</formula>
+      <formula>$A6&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:F1">
@@ -1213,8 +1220,11 @@
       <formula>"削除"</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="C13" r:id="rId1" xr:uid="{1D7FDBB9-ABBE-4A13-BDF5-75DB9BF79937}"/>
+  </hyperlinks>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="8" scale="51" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="8" scale="51" orientation="portrait" r:id="rId2"/>
   <headerFooter>
     <oddFooter>&amp;R&amp;Z&amp;F</oddFooter>
   </headerFooter>

</xml_diff>